<commit_message>
Shear Wavy Simulation + createGeometry
A simulation with attempt to recreate Gaussian distribution in k vs lambda space and parameterization of geometry creation in Abaqus.
</commit_message>
<xml_diff>
--- a/Data_Inventory.xlsx
+++ b/Data_Inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CD2F46-662E-4B1D-A9DE-8D079144FF32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F29F6C-743D-4FF7-A1F0-08E493C94036}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>UMItools</t>
   </si>
@@ -234,6 +234,21 @@
   </si>
   <si>
     <t>Geometry created within matlab (input commands are in DefGrad_sim_v8, see ReadMe.txt)</t>
+  </si>
+  <si>
+    <t>Plot2DHists_ShearWavy</t>
+  </si>
+  <si>
+    <t>Create Gaussian decomposition histograms</t>
+  </si>
+  <si>
+    <t>ogdenShearVSI-data\Decomposition_Sensititivity\22-1212-Shear_Wavy\sensitivity.mat</t>
+  </si>
+  <si>
+    <t>ogdenShearVSI-data\Decomposition_Sensititivity\22-12-Shear_Wavy (Folder)</t>
+  </si>
+  <si>
+    <t>2D histograms of k vs lam for wavy shear simulation</t>
   </si>
 </sst>
 </file>
@@ -770,13 +785,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,90 +959,111 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
       <c r="B9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="9" t="s">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="11"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Parametric sweep and entropy calculations
Various parametric sweeps of the shear wavy sample (sin amplitude, sin periods, width of samples) and results. Note: some files are missing [too big], so you'll have to run locally to reproduce them.
</commit_message>
<xml_diff>
--- a/Data_Inventory.xlsx
+++ b/Data_Inventory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CF0130-837A-4FF7-A967-26C473B1BAC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7378DC27-DAAE-4171-A9F8-52ACCD98A845}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>UMItools</t>
   </si>
@@ -248,19 +248,22 @@
     <t>Same as runComplexFilter_Ogden and DefGrad_sim_v9 outputs</t>
   </si>
   <si>
-    <t>Plot2DHists_WavySweep</t>
-  </si>
-  <si>
-    <t>ogdenShearVSI-data\Decomposition_Sensititivity\22-1215-Wavy_sweep\sensitivity.mat</t>
-  </si>
-  <si>
     <t>ogdenShearVSI-data\Decomposition_Sensititivity\22-1212-Shear_Wavy (Folder)</t>
   </si>
   <si>
-    <t>ogdenShearVSI-data\Decomposition_Sensititivity\22-1215-Wavy_Sweep (Folder)</t>
-  </si>
-  <si>
     <t>Geometry created within matlab (input commands are in DefGrad_sim_v9, see ReadMe.txt)</t>
+  </si>
+  <si>
+    <t>ogdenShearVSI-data\Decomposition_Sensititivity\[Data_Wavy-Thick_Amp/Prd/Width]_Sweep\sensitivity.mat</t>
+  </si>
+  <si>
+    <t>ogdenShearVSI-data\Decomposition_Sensititivity\[Data_Wavy-Thick_Amp/Prd/Width]_Sweep (Folder)</t>
+  </si>
+  <si>
+    <t>Plot2DHists_Sweep</t>
+  </si>
+  <si>
+    <t>2D histograms/entropy plots of k vs lam for any parameteric sweep simulation</t>
   </si>
 </sst>
 </file>
@@ -800,10 +803,10 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +909,7 @@
         <v>50</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>51</v>
@@ -986,7 +989,7 @@
         <v>34</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>58</v>
@@ -995,13 +998,13 @@
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1010,7 +1013,7 @@
         <v>63</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">

</xml_diff>